<commit_message>
update xls page num formatting.
</commit_message>
<xml_diff>
--- a/sec542/SEC542.xlsx
+++ b/sec542/SEC542.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Page</t>
   </si>
@@ -19,13 +19,19 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>Notes</t>
+    <t>Page Content Overview</t>
+  </si>
+  <si>
+    <t>1-5</t>
   </si>
   <si>
     <t>why web applications, why, xss, sqli</t>
   </si>
   <si>
     <t>web apps are popular because of widespread use.  extremely portable.  range of OS platforms.  stores, manages, and access sensitive info</t>
+  </si>
+  <si>
+    <t>1-6</t>
   </si>
   <si>
     <t>tangled web, zalewski, design, security</t>
@@ -40,10 +46,16 @@
     <t>all browsers support http 0.9</t>
   </si>
   <si>
+    <t>1-7</t>
+  </si>
+  <si>
     <t>security testing, development, software, national vulnerability database, exploit database, offensive security, http://nvd.nist.gof, http://www.xssed.com, http://ww.exploit-db.com</t>
   </si>
   <si>
     <t>xssed announces public websites being found vulnerable to various flaws (no longer actively maintained).</t>
+  </si>
+  <si>
+    <t>1-8</t>
   </si>
   <si>
     <t>web 2.0, http, ajax, google maps</t>
@@ -52,10 +64,16 @@
     <t>web 2.0 is overused and annoying, pages can be dynamically updated with ajax, google maps is a good example of ajax interaction</t>
   </si>
   <si>
+    <t>1-9</t>
+  </si>
+  <si>
     <t>cloud, on-demand resources, liability, restriction, vendors</t>
   </si>
   <si>
     <t>vendors hesitate to allow testing or so its assumed, liability limits testing.  same types of risks and flaws as non-cloud based services.  many cloud vendors allow testing, you just have to ask</t>
+  </si>
+  <si>
+    <t>1-11</t>
   </si>
   <si>
     <t>pen testers viewpoint, viewpoint, pen testers, mistakes</t>
@@ -64,10 +82,16 @@
     <t>must think maliciously, but act professionally, what mistakes did the developers make?</t>
   </si>
   <si>
+    <t>1-12</t>
+  </si>
+  <si>
     <t>penetration testing, vulnerability disovery, methodology, pen testing methodology, typical pen testing methodology, service-side pen test, client-side pen test, OWASP, PTES, penetration testing execution standard, methodologies</t>
   </si>
   <si>
     <t>typical methodology is too rigid:  Recon, scanning, vuln testing, exploit, post exploit, reporting.   client-side pen test: means the victim initiates the connection, service-side pen test: means the pen tester initiates the connection.  web app pen testers tend to be much more fluid:  once discovery of sqli we tend to go for the kill immediately.  PTES (penetration testing execution standard) offers great starting point.  OWASP matches up best for web pen tests, http://www.pentest-standard.org/</t>
+  </si>
+  <si>
+    <t>1-13</t>
   </si>
   <si>
     <t>OWASP, OTG, OWASP Testing Guide, test ids, OWASP test ids, testing checklist, checklist, OWASP Testing Project</t>
@@ -80,9 +104,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m-d"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -134,7 +155,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -213,102 +234,102 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="5">
-        <v>42740.0</v>
+      <c r="A2" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
-        <v>42741.0</v>
+      <c r="A3" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5">
-        <v>42741.0</v>
-      </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
-        <v>42742.0</v>
+      <c r="A5" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
-        <v>42743.0</v>
+      <c r="A6" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
-        <v>42744.0</v>
+      <c r="A7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5">
-        <v>42746.0</v>
+      <c r="A8" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5">
-        <v>42747.0</v>
+      <c r="A9" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5">
-        <v>42748.0</v>
+      <c r="A10" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">

</xml_diff>